<commit_message>
excel sheet change: :
</commit_message>
<xml_diff>
--- a/assets/canadianMentalHealthResources.xlsx
+++ b/assets/canadianMentalHealthResources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://queensuca-my.sharepoint.com/personal/23nrd2_queensu_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEFDB21-0B4B-4144-B833-9360189A904F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA43D6BE-5F28-4BD0-82D5-BBB14C904E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16980" xr2:uid="{60D886F8-FFE1-F14E-A3CB-AFDAAB1FA1C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="660">
   <si>
     <t>Province</t>
   </si>
@@ -2060,6 +2060,21 @@
   </si>
   <si>
     <t>1-800-668-6868 or text “CONNECT” to 686868</t>
+  </si>
+  <si>
+    <t>552 Princess Street, Kingston, ON</t>
+  </si>
+  <si>
+    <t>Addiction &amp; Mental Health Services – KFLA (AMHS-KFLA)</t>
+  </si>
+  <si>
+    <t>Provides mental health and addiction support services in the Kingston, Frontenac, Lennox, and Addington areas</t>
+  </si>
+  <si>
+    <t>613-544-1356</t>
+  </si>
+  <si>
+    <t>https://amhs-kfla.ca/</t>
   </si>
 </sst>
 </file>
@@ -2194,7 +2209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2219,6 +2234,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2554,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8E0B34-D33C-AB4E-A291-CAA443D46446}">
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F45" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="F146" workbookViewId="0">
+      <selection activeCell="J154" sqref="J154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6791,6 +6809,38 @@
       </c>
       <c r="K153" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
+      <c r="A154" t="s">
+        <v>386</v>
+      </c>
+      <c r="B154" t="s">
+        <v>450</v>
+      </c>
+      <c r="C154" t="s">
+        <v>655</v>
+      </c>
+      <c r="D154" t="s">
+        <v>12</v>
+      </c>
+      <c r="E154" t="s">
+        <v>656</v>
+      </c>
+      <c r="F154" t="s">
+        <v>657</v>
+      </c>
+      <c r="G154" t="s">
+        <v>658</v>
+      </c>
+      <c r="H154" s="13" t="s">
+        <v>659</v>
+      </c>
+      <c r="I154" s="18">
+        <v>44.233800000000002</v>
+      </c>
+      <c r="J154">
+        <v>76.497299999999996</v>
       </c>
     </row>
   </sheetData>
@@ -6903,6 +6953,7 @@
     <hyperlink ref="H63" r:id="rId106" xr:uid="{B442E89A-EC9B-4ECB-87C7-2C2244E59EBC}"/>
     <hyperlink ref="H64" r:id="rId107" xr:uid="{C3C976CD-1869-46C4-BCCA-0B261A8272FD}"/>
     <hyperlink ref="H65" r:id="rId108" xr:uid="{BDBFBA04-C3F5-49E3-A03E-7A400D4278D8}"/>
+    <hyperlink ref="H154" r:id="rId109" xr:uid="{3EE46F70-8110-4047-85AF-DBA27F8BB891}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>